<commit_message>
The following untracked working tree files would be overwritten by merge
</commit_message>
<xml_diff>
--- a/Test case/Логотип на ручке..xlsx
+++ b/Test case/Логотип на ручке..xlsx
@@ -108,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -157,60 +157,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -226,20 +177,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -248,16 +189,11 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +502,7 @@
   <dimension ref="A3:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A18"/>
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,30 +517,30 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
@@ -613,160 +549,174 @@
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B20:C20"/>
@@ -778,20 +728,6 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>